<commit_message>
Modificaciones y requisitos minimos
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -49,10 +49,7 @@
     <t xml:space="preserve">R01</t>
   </si>
   <si>
-    <t xml:space="preserve">sdfsdfsdfsdfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skdjfksjf skjf hskjfh kjsdh fkjs hkjh fdjksh fkjsdh fkjs dfkjs dfkj sjkd fsjk fkjs fkjs fkjs fjks fjks hfkjs fjks hfjks hfjks hfjks hfjk sfjks fjks hfjks hjkf hsjkfs jk</t>
+    <t xml:space="preserve">Utilizar las etiquetas semánticas de HTML5</t>
   </si>
   <si>
     <t xml:space="preserve">Mínimo</t>
@@ -70,67 +67,175 @@
     <t xml:space="preserve">R02</t>
   </si>
   <si>
-    <t xml:space="preserve">kdldjflgdfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdlksdljkfsldjfsd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importante</t>
+    <t xml:space="preserve">Presentación mediante CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño flexible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existencia de transiciones, transformaciones, animaciones y contenido multimedia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de microdatos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Superar: Validador de HTML5 y CSS3, Nivel de accesibilidad AA, Prueba del Seis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar el diseño para resoluciones grandes y pequeñas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprobar que el diseño es correcto es diferentes navegadores: Internet Explorer, Chrome, Mozila Firefox y Opera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de PHP 7.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de Yii2 Framework versión 2.0.10 o superior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de PostgreSQL versión 9.6 o superior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despliegue de la aplicación en la plataforma Heroku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pruebas funcionales con Codeception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estilo y mantenibilidad del código fuente validados por Code Climate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño escalable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de AJAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilización de mecanismos de comunicación asíncrona.</t>
   </si>
   <si>
     <t xml:space="preserve">v2</t>
   </si>
   <si>
-    <t xml:space="preserve">R03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdfsfd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lkcvlkjxcjklcxljkwejlksdfvc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Información</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sfsfsfd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jk34jlk4n,lkjlksdflksdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opcional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funcional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xcvxcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdkfjklsdfjldksf
-- sdlkfjlksdjfldksjflksjfdss
-- slkdjflksjflksjflksjkljfksldjfldks
-sldkjflskdjfdlskjflksdjflkdsjflkjslkfjslkjfdlskjflsjklfdjslkjlskjdflks
-klsdjfkljsdlkfjskldf
-sdklfjklsdjfklsdjflksdjfklsdjkl
-lñklllllllllllllllllllllllqweqweqweqew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difícil</t>
+    <t xml:space="preserve">R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validación de campos en formularios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de ventanas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestión de la apariencia de las ventanas. Creación de nuevas ventanas y comunicación entre ventanas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactividad  a través de mecanismos de manejo de eventos intuitivos y eficaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso y manipulación del DOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de mecanismos de almacenamiento en el lado del cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de jQuery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incluir al menos un plugin no trabajado en clase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despliegue en un Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar un despliegue en un servidor local usando y configurando  tres máquinas virtuales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear un servicio de Nombres de dominio.
+Gestionar y administrar el servidor Apache tanto en Windows como Linux:
+- Instalar el servidor y configurarlo.
+- Configurar directivas.
+- Usar directorios virtuales y redireccionamientos.
+- Usar diferentes módulos estáticos y dinámicos.
+- Usar autenticaciones.
+- Usar ficheros de configuración personalizada de directorios.
+- Usar HTTPS y certificados Digitales.
+</t>
   </si>
 </sst>
 </file>
@@ -270,19 +375,19 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -318,112 +423,526 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="G5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="8" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="64.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="79.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="33.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>24</v>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="136.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -445,7 +964,7 @@
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D6" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D6:D27" type="list">
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -465,7 +984,7 @@
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6:E27" type="list">
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -485,7 +1004,7 @@
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F6" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F6:F27" type="list">
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -505,7 +1024,7 @@
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G6" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G6:G27" type="list">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Anadiendo requisitos a la propuesta
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="139">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -218,6 +218,11 @@
   </si>
   <si>
     <t xml:space="preserve">Despliegue en un Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Utilizando algún servicio gratuito de hosting como los vistos en clase 
+- Instalar / configurar o solicitar el software necesario para desplegar el proyecto.
+</t>
   </si>
   <si>
     <t xml:space="preserve">R26</t>
@@ -237,6 +242,224 @@
 - Usar HTTPS y certificados Digitales.
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">R27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar un diseño de cada página de la aplicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Diseño corporativo general
+- Diseño de página de inicio
+- Diseño de página de información sobre el equipo y sus jugadores
+- Diseño de página del calendario
+- Diseño de páginas para unirse al equipo o luchar contra él
+- Diseño de página de normas
+- Diseño de página de política de cookies
+- Diseño de página de políticas de privacidad
+- Diseño de página de torneos
+- Diseño de página del perfil del usuario
+- Diseño de página de noticia
+- Diseño de página del panel de administrador y usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudio sobre palabras clave de búsqueda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilización de la herramienta Kwfinder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Información</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difícil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartir un enlace de entrenamiento del calendario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando un administrador crea un evento en el calendario de tipo entrenamiento se creará un enlace para compartirlo. El administrador lo compartirá con los integrantes del equipo para que puedan participar en el evento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opcional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunicar API de twitter con la aplicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunicar API de twitch con la aplicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dar de alta a usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solo lo pueden realizar los administradores desde el back-end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dar de baja a usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solo lo pueden realizar los administradores desde el back-end. Se tienen que borrar todos los datos sensibles del usuario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador puede cambiar el rol de un usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferenciar Usuarios normales a usuarios en prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Establecer distintos roles a los usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada rol tiene un permiso/visibilidad asociado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expulsar a un usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expulsa de manera temporal a un usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login y cierre de sesión de un usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correo de confirmación de un usuario nuevo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador enviará un correo con en el enlace de invitación y un código de verificación en el cuerpo del mensaje al nuevo usuario desde el panel. El usuario accederá al enlace y verificará su identidad con el código del mensaje. De manera que pueda crear su propia cuenta con credenciales a continuación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseñar una plantilla HTML para los correos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear una cuenta de usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiene que aceptar tanto las normas del equipo como la política de privacidad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedir una invitación al equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A través de un formulario. Envía un correo al administrador. Además de que aparezca en el panel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedir una lucha entre equipos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver información relevante de los integrantes del equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realizará a través de la API de Clash Royale para recibir los datos. Estos se cachearán en la BD de la aplicación para agilizar el proceso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración de cuentas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credenciales para acceder a twitter y twitch, cambiar información relevante a la cuenta del administrador.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quitar expulsión de usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar batallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra de forma dinámica las batallas de los jugadores con un poco de información sobre ellas. Se le asociará además un rol de visibilidad con el que puedan mostrarse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar vídeos de twitch a batallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador proporcionará un enlace del vídeo de la cuenta de twitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocultar batallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oculta la batalla para que no se pueda ver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear un torneo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para crearlo el administrador proporcionará un tag de torneo (está en la app) válido</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +468,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -275,6 +498,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -319,7 +548,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -356,6 +585,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -375,19 +612,20 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F53" activeCellId="0" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="66.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="11.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -423,6 +661,7 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="0"/>
       <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
@@ -443,6 +682,7 @@
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="C3" s="0"/>
       <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
@@ -463,6 +703,7 @@
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C4" s="0"/>
       <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
@@ -483,6 +724,7 @@
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C5" s="0"/>
       <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
@@ -503,6 +745,7 @@
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C6" s="0"/>
       <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
@@ -510,7 +753,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>23</v>
@@ -523,6 +766,7 @@
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C7" s="0"/>
       <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
@@ -543,6 +787,7 @@
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C8" s="0"/>
       <c r="D8" s="8" t="s">
         <v>10</v>
       </c>
@@ -563,6 +808,7 @@
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C9" s="0"/>
       <c r="D9" s="8" t="s">
         <v>10</v>
       </c>
@@ -583,6 +829,7 @@
       <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C10" s="0"/>
       <c r="D10" s="8" t="s">
         <v>10</v>
       </c>
@@ -603,6 +850,7 @@
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C11" s="0"/>
       <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
@@ -623,6 +871,7 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="C12" s="0"/>
       <c r="D12" s="8" t="s">
         <v>10</v>
       </c>
@@ -643,6 +892,7 @@
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C13" s="0"/>
       <c r="D13" s="8" t="s">
         <v>10</v>
       </c>
@@ -663,6 +913,7 @@
       <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C14" s="0"/>
       <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
@@ -683,6 +934,7 @@
       <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="C15" s="0"/>
       <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
@@ -703,6 +955,7 @@
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C16" s="0"/>
       <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
@@ -723,6 +976,7 @@
       <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="C17" s="0"/>
       <c r="D17" s="8" t="s">
         <v>10</v>
       </c>
@@ -766,6 +1020,7 @@
       <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C19" s="0"/>
       <c r="D19" s="8" t="s">
         <v>10</v>
       </c>
@@ -809,6 +1064,7 @@
       <c r="B21" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="C21" s="0"/>
       <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
@@ -829,6 +1085,7 @@
       <c r="B22" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="C22" s="0"/>
       <c r="D22" s="8" t="s">
         <v>10</v>
       </c>
@@ -849,6 +1106,7 @@
       <c r="B23" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="C23" s="0"/>
       <c r="D23" s="8" t="s">
         <v>10</v>
       </c>
@@ -869,6 +1127,7 @@
       <c r="B24" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="C24" s="0"/>
       <c r="D24" s="8" t="s">
         <v>10</v>
       </c>
@@ -889,6 +1148,7 @@
       <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="C25" s="0"/>
       <c r="D25" s="8" t="s">
         <v>10</v>
       </c>
@@ -902,13 +1162,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="34.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="C26" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="D26" s="8" t="s">
         <v>10</v>
       </c>
@@ -922,15 +1185,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="136.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>10</v>
@@ -943,6 +1206,537 @@
       </c>
       <c r="G27" s="8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -964,7 +1758,7 @@
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D6:D27" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D6:D51" type="list">
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -984,7 +1778,7 @@
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6:E27" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6:E51" type="list">
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1004,7 +1798,7 @@
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F6:F27" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F6:F51" type="list">
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1024,7 +1818,7 @@
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G6:G27" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G6:G51" type="list">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>